<commit_message>
Correcting errors in trial matrix and code
</commit_message>
<xml_diff>
--- a/Stimulus/TrialMatrix_LM2.xlsx
+++ b/Stimulus/TrialMatrix_LM2.xlsx
@@ -129,10 +129,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D194"/>
+  <dimension ref="A1:D1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A166" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B205" activeCellId="0" sqref="B205"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A121" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A140" activeCellId="0" sqref="A140"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2088,18 +2088,18 @@
         <v>4</v>
       </c>
     </row>
-    <row r="140" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="140" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A140" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B140" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C140" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D140" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="141" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2110,10 +2110,10 @@
         <v>2</v>
       </c>
       <c r="C141" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D141" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="142" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2121,13 +2121,13 @@
         <v>0</v>
       </c>
       <c r="B142" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C142" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D142" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="143" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2138,10 +2138,10 @@
         <v>1</v>
       </c>
       <c r="C143" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D143" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2149,13 +2149,13 @@
         <v>0</v>
       </c>
       <c r="B144" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C144" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D144" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="145" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2163,13 +2163,13 @@
         <v>0</v>
       </c>
       <c r="B145" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C145" s="0" t="n">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="D145" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="146" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2180,10 +2180,10 @@
         <v>1</v>
       </c>
       <c r="C146" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="D146" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="147" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2191,10 +2191,10 @@
         <v>0</v>
       </c>
       <c r="B147" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C147" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
       <c r="D147" s="0" t="n">
         <v>8</v>
@@ -2208,10 +2208,10 @@
         <v>2</v>
       </c>
       <c r="C148" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D148" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
     </row>
     <row r="149" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2222,10 +2222,10 @@
         <v>2</v>
       </c>
       <c r="C149" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D149" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="150" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2233,13 +2233,13 @@
         <v>0</v>
       </c>
       <c r="B150" s="0" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C150" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
       <c r="D150" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="151" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2250,10 +2250,10 @@
         <v>1</v>
       </c>
       <c r="C151" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D151" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
     </row>
     <row r="152" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2261,13 +2261,13 @@
         <v>0</v>
       </c>
       <c r="B152" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C152" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D152" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="153" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2275,13 +2275,13 @@
         <v>0</v>
       </c>
       <c r="B153" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C153" s="0" t="n">
         <v>4</v>
       </c>
       <c r="D153" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="154" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2292,10 +2292,10 @@
         <v>2</v>
       </c>
       <c r="C154" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D154" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="155" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2303,13 +2303,13 @@
         <v>0</v>
       </c>
       <c r="B155" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C155" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D155" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="156" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2320,10 +2320,10 @@
         <v>3</v>
       </c>
       <c r="C156" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D156" s="0" t="n">
-        <v>10</v>
+        <v>2</v>
       </c>
     </row>
     <row r="157" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2334,10 +2334,10 @@
         <v>3</v>
       </c>
       <c r="C157" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D157" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="158" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2345,13 +2345,13 @@
         <v>0</v>
       </c>
       <c r="B158" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C158" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D158" s="0" t="n">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="159" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2359,13 +2359,13 @@
         <v>0</v>
       </c>
       <c r="B159" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C159" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D159" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2373,13 +2373,13 @@
         <v>0</v>
       </c>
       <c r="B160" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C160" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D160" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="161" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2401,13 +2401,13 @@
         <v>0</v>
       </c>
       <c r="B162" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C162" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D162" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="163" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2418,10 +2418,10 @@
         <v>2</v>
       </c>
       <c r="C163" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="D163" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="164" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2429,13 +2429,13 @@
         <v>0</v>
       </c>
       <c r="B164" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C164" s="0" t="n">
         <v>8</v>
       </c>
       <c r="D164" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2443,13 +2443,13 @@
         <v>0</v>
       </c>
       <c r="B165" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C165" s="0" t="n">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="D165" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2457,13 +2457,13 @@
         <v>0</v>
       </c>
       <c r="B166" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C166" s="0" t="n">
         <v>2</v>
       </c>
       <c r="D166" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="167" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2474,10 +2474,10 @@
         <v>3</v>
       </c>
       <c r="C167" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D167" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2485,10 +2485,10 @@
         <v>0</v>
       </c>
       <c r="B168" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C168" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D168" s="0" t="n">
         <v>2</v>
@@ -2499,13 +2499,13 @@
         <v>0</v>
       </c>
       <c r="B169" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C169" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="D169" s="0" t="n">
-        <v>2</v>
+        <v>8</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2513,10 +2513,10 @@
         <v>0</v>
       </c>
       <c r="B170" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C170" s="0" t="n">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="D170" s="0" t="n">
         <v>8</v>
@@ -2533,7 +2533,7 @@
         <v>2</v>
       </c>
       <c r="D171" s="0" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2541,13 +2541,13 @@
         <v>0</v>
       </c>
       <c r="B172" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C172" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="D172" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="173" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2555,13 +2555,13 @@
         <v>0</v>
       </c>
       <c r="B173" s="0" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C173" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D173" s="0" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="174" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2569,13 +2569,13 @@
         <v>0</v>
       </c>
       <c r="B174" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C174" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D174" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="175" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2583,13 +2583,13 @@
         <v>0</v>
       </c>
       <c r="B175" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C175" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="D175" s="0" t="n">
-        <v>8</v>
+        <v>4</v>
       </c>
     </row>
     <row r="176" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2597,13 +2597,13 @@
         <v>0</v>
       </c>
       <c r="B176" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C176" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D176" s="0" t="n">
-        <v>4</v>
+        <v>8</v>
       </c>
     </row>
     <row r="177" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2614,10 +2614,10 @@
         <v>2</v>
       </c>
       <c r="C177" s="0" t="n">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D177" s="0" t="n">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="178" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2628,10 +2628,10 @@
         <v>2</v>
       </c>
       <c r="C178" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D178" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="179" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2639,13 +2639,13 @@
         <v>0</v>
       </c>
       <c r="B179" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C179" s="0" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="D179" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="180" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2653,13 +2653,13 @@
         <v>0</v>
       </c>
       <c r="B180" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C180" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D180" s="0" t="n">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="181" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2670,10 +2670,10 @@
         <v>1</v>
       </c>
       <c r="C181" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D181" s="0" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="182" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2681,13 +2681,13 @@
         <v>0</v>
       </c>
       <c r="B182" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C182" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D182" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="183" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2695,13 +2695,13 @@
         <v>0</v>
       </c>
       <c r="B183" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C183" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="D183" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
     </row>
     <row r="184" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2709,13 +2709,13 @@
         <v>0</v>
       </c>
       <c r="B184" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C184" s="0" t="n">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="D184" s="0" t="n">
-        <v>10</v>
+        <v>4</v>
       </c>
     </row>
     <row r="185" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2726,7 +2726,7 @@
         <v>1</v>
       </c>
       <c r="C185" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
       <c r="D185" s="0" t="n">
         <v>4</v>
@@ -2740,10 +2740,10 @@
         <v>1</v>
       </c>
       <c r="C186" s="0" t="n">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="D186" s="0" t="n">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2754,10 +2754,10 @@
         <v>1</v>
       </c>
       <c r="C187" s="0" t="n">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="D187" s="0" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2765,13 +2765,13 @@
         <v>0</v>
       </c>
       <c r="B188" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C188" s="0" t="n">
-        <v>0</v>
+        <v>10</v>
       </c>
       <c r="D188" s="0" t="n">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2779,13 +2779,13 @@
         <v>0</v>
       </c>
       <c r="B189" s="0" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C189" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D189" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2793,13 +2793,13 @@
         <v>0</v>
       </c>
       <c r="B190" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C190" s="0" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="D190" s="0" t="n">
-        <v>2</v>
+        <v>10</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2807,10 +2807,10 @@
         <v>0</v>
       </c>
       <c r="B191" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C191" s="0" t="n">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D191" s="0" t="n">
         <v>10</v>
@@ -2821,13 +2821,13 @@
         <v>0</v>
       </c>
       <c r="B192" s="0" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="C192" s="0" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="D192" s="0" t="n">
-        <v>10</v>
+        <v>6</v>
       </c>
     </row>
     <row r="193" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2835,29 +2835,16 @@
         <v>0</v>
       </c>
       <c r="B193" s="0" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C193" s="0" t="n">
         <v>10</v>
       </c>
       <c r="D193" s="0" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="194" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A194" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="B194" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C194" s="0" t="n">
-        <v>10</v>
-      </c>
-      <c r="D194" s="0" t="n">
-        <v>0</v>
-      </c>
-    </row>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>